<commit_message>
add date column to tests
</commit_message>
<xml_diff>
--- a/tests/Feature/ExportTest/simple_dummies.xlsx
+++ b/tests/Feature/ExportTest/simple_dummies.xlsx
@@ -15,12 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>date_time</t>
   </si>
   <si>
     <t>test 1</t>
@@ -36,7 +39,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd.mm.yyyy"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <b val="0"/>
@@ -53,10 +58,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -65,12 +67,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="1" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -367,53 +375,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="true" style="1"/>
     <col min="2" max="2" width="16" customWidth="true" style="0"/>
+    <col min="3" max="3" width="16" customWidth="true" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43831.0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43831.0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43831.0</v>
       </c>
     </row>
   </sheetData>
@@ -429,5 +450,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>